<commit_message>
Cập nhật route danh sách, xóa, xuất Excel và template danh_sach_yeu_cau
</commit_message>
<xml_diff>
--- a/yeu_cau_cong_viec.xlsx
+++ b/yeu_cau_cong_viec.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,222 +495,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>04/07/2025</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Kế Toán</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Lỗi mạng internet</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Dũng</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>04/07/2025</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Phòng Điều dưỡng</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Lỗi HIS</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>250008971</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2500000014</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>báo sai thông tin</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Đặng Văn Thạch</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Thạch</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>04/07/2025</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Khoa Ba chuyên khoa</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Lỗi LIS(XN)</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>250008971</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2500000014</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>srgdhadfhdghfgfg</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Lê Tú Thanh Trinh</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>anh</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>04/07/2025</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Khoa Ba chuyên khoa</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Lỗi mạng internet</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>máy tính không vào mạng được</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Nguyễn Thị Cẩm Linh</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Linh</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>✗</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>